<commit_message>
240816-1024 Timer Process Closer Repair, Add Function
</commit_message>
<xml_diff>
--- a/TimerProcessCloser/TimerProcessCloser_docs/TimerProcessCloser.xlsx
+++ b/TimerProcessCloser/TimerProcessCloser_docs/TimerProcessCloser.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="30" windowWidth="19200" windowHeight="12090" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="30" windowWidth="19200" windowHeight="12090"/>
   </bookViews>
   <sheets>
     <sheet name="概要_機能" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="220">
   <si>
     <t>■概要</t>
     <rPh sb="1" eb="3">
@@ -1085,28 +1085,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>アプリの終了だけでなく、コマンドの実行にも対応（コマンド入力欄、アクション設定欄が必要）</t>
-    <rPh sb="4" eb="6">
-      <t>シュウリョウ</t>
-    </rPh>
-    <rPh sb="17" eb="19">
-      <t>ジッコウ</t>
-    </rPh>
-    <rPh sb="21" eb="23">
-      <t>タイオウ</t>
-    </rPh>
-    <rPh sb="28" eb="31">
-      <t>ニュウリョクラン</t>
-    </rPh>
-    <rPh sb="37" eb="40">
-      <t>セッテイラン</t>
-    </rPh>
-    <rPh sb="41" eb="43">
-      <t>ヒツヨウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>画面更新</t>
     <rPh sb="0" eb="4">
       <t>ガメンコウシン</t>
@@ -1207,28 +1185,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>&gt;&gt;入力情報の簡略化、現状で1時間を入力するには"1:00:00"をすべて入力しなければならない。</t>
-    <rPh sb="2" eb="6">
-      <t>ニュウリョクジョウホウ</t>
-    </rPh>
-    <rPh sb="7" eb="10">
-      <t>カンリャクカ</t>
-    </rPh>
-    <rPh sb="11" eb="13">
-      <t>ゲンジョウ</t>
-    </rPh>
-    <rPh sb="15" eb="17">
-      <t>ジカン</t>
-    </rPh>
-    <rPh sb="18" eb="20">
-      <t>ニュウリョク</t>
-    </rPh>
-    <rPh sb="37" eb="39">
-      <t>ニュウリョク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>機能修正：Release版で、ログファイルが正しく設定されない修正</t>
     <rPh sb="0" eb="4">
       <t>キノウシュウセイ</t>
@@ -1896,25 +1852,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>&gt;&gt;完了前通知は、アイテムごとに設定変更可能にする（コントロールパーツの追加が必要）（または詳細設定欄を設ける？）</t>
-    <rPh sb="2" eb="7">
-      <t>カンリョウマエツウチ</t>
-    </rPh>
-    <rPh sb="36" eb="38">
-      <t>ツイカ</t>
-    </rPh>
-    <rPh sb="39" eb="41">
-      <t>ヒツヨウ</t>
-    </rPh>
-    <rPh sb="46" eb="51">
-      <t>ショウサイセッテイラン</t>
-    </rPh>
-    <rPh sb="52" eb="53">
-      <t>モウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>終了させてはいけないプロセス名（explorer, svchost、cmd.exeなど）を設定する（設定時はエラーダイアログ表示して、入力を抑止）</t>
     <rPh sb="0" eb="2">
       <t>シュウリョウ</t>
@@ -1981,24 +1918,269 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>&gt;&gt;タイマー停止については、状態名を追加して、個別の処理も追加する。</t>
+    <t>タイマー終了時の実行処理にプロセスの起動を追加</t>
+    <rPh sb="4" eb="7">
+      <t>シュウリョウジ</t>
+    </rPh>
+    <rPh sb="8" eb="12">
+      <t>ジッコウショリ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>キドウ</t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t>ツイカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>アプリ名・プロジェクト名の変更は検討中</t>
+    <rPh sb="3" eb="4">
+      <t>メイ</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>メイ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>ヘンコウ</t>
+    </rPh>
+    <rPh sb="16" eb="19">
+      <t>ケントウチュウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>必要タスク・未完了（仕様書の修正、手順、手順画像、機能、保存用ファイル）</t>
+    <rPh sb="0" eb="2">
+      <t>ヒツヨウ</t>
+    </rPh>
+    <rPh sb="6" eb="9">
+      <t>ミカンリョウ</t>
+    </rPh>
+    <rPh sb="10" eb="13">
+      <t>シヨウショ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>シュウセイ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>テジュン</t>
+    </rPh>
+    <rPh sb="20" eb="24">
+      <t>テジュンガゾウ</t>
+    </rPh>
+    <rPh sb="25" eb="27">
+      <t>キノウ</t>
+    </rPh>
+    <rPh sb="28" eb="31">
+      <t>ホゾンヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>■新画面 240816</t>
+    <rPh sb="1" eb="2">
+      <t>シン</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ガメン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>アプリの終了だけでなく、コマンドの実行にも対応（コマンド入力欄、アクション設定欄が必要）（済240816）</t>
+    <rPh sb="4" eb="6">
+      <t>シュウリョウ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>ジッコウ</t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t>タイオウ</t>
+    </rPh>
+    <rPh sb="28" eb="31">
+      <t>ニュウリョクラン</t>
+    </rPh>
+    <rPh sb="37" eb="40">
+      <t>セッテイラン</t>
+    </rPh>
+    <rPh sb="41" eb="43">
+      <t>ヒツヨウ</t>
+    </rPh>
+    <rPh sb="45" eb="46">
+      <t>スミ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>タイマー完了時のアクションがプロセス実行の時、プロセス名が長すぎて見切れる対処、オプション引数はどうするかは要検討する</t>
+    <rPh sb="4" eb="7">
+      <t>カンリョウジ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>ジッコウ</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>トキ</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>メイ</t>
+    </rPh>
+    <rPh sb="29" eb="30">
+      <t>ナガ</t>
+    </rPh>
+    <rPh sb="33" eb="35">
+      <t>ミキ</t>
+    </rPh>
+    <rPh sb="37" eb="39">
+      <t>タイショ</t>
+    </rPh>
+    <rPh sb="45" eb="47">
+      <t>ヒキスウ</t>
+    </rPh>
+    <rPh sb="54" eb="55">
+      <t>ヨウ</t>
+    </rPh>
+    <rPh sb="55" eb="57">
+      <t>ケントウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>　&gt;&gt;完了前通知は、アイテムごとに設定変更可能にする（コントロールパーツの追加が必要）（または詳細設定欄を設ける？）</t>
+    <rPh sb="3" eb="8">
+      <t>カンリョウマエツウチ</t>
+    </rPh>
+    <rPh sb="37" eb="39">
+      <t>ツイカ</t>
+    </rPh>
+    <rPh sb="40" eb="42">
+      <t>ヒツヨウ</t>
+    </rPh>
+    <rPh sb="47" eb="52">
+      <t>ショウサイセッテイラン</t>
+    </rPh>
+    <rPh sb="53" eb="54">
+      <t>モウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>　&gt;&gt;入力情報の簡略化、現状で1時間を入力するには"1:00:00"をすべて入力しなければならない。</t>
+    <rPh sb="3" eb="7">
+      <t>ニュウリョクジョウホウ</t>
+    </rPh>
+    <rPh sb="8" eb="11">
+      <t>カンリャクカ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>ゲンジョウ</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>ジカン</t>
+    </rPh>
+    <rPh sb="19" eb="21">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="38" eb="40">
+      <t>ニュウリョク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>　&gt;&gt;タイマー停止については、状態名を追加して、個別の処理も追加する。</t>
+    <rPh sb="7" eb="9">
+      <t>テイシ</t>
+    </rPh>
+    <rPh sb="15" eb="18">
+      <t>ジョウタイメイ</t>
+    </rPh>
+    <rPh sb="19" eb="21">
+      <t>ツイカ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>コベツ</t>
+    </rPh>
+    <rPh sb="27" eb="29">
+      <t>ショリ</t>
+    </rPh>
+    <rPh sb="30" eb="32">
+      <t>ツイカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>*****</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>修正：アプリ終了時に、コンボボックス通知とActionが正しくSetting.xmlに保存されていない修正</t>
+    <rPh sb="0" eb="2">
+      <t>シュウセイ</t>
+    </rPh>
+    <rPh sb="6" eb="9">
+      <t>シュウリョウジ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>ツウチ</t>
+    </rPh>
+    <rPh sb="28" eb="29">
+      <t>タダ</t>
+    </rPh>
+    <rPh sb="43" eb="45">
+      <t>ホゾン</t>
+    </rPh>
+    <rPh sb="51" eb="53">
+      <t>シュウセイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>3-2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>3-1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>プロセスの実行/終了</t>
+    <rPh sb="5" eb="7">
+      <t>ジッコウ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>シュウリョウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>プロセス実行機能</t>
+    <rPh sb="4" eb="6">
+      <t>ジッコウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>240816機能追加</t>
     <rPh sb="6" eb="8">
-      <t>テイシ</t>
-    </rPh>
-    <rPh sb="14" eb="17">
-      <t>ジョウタイメイ</t>
-    </rPh>
-    <rPh sb="18" eb="20">
+      <t>キノウ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
       <t>ツイカ</t>
     </rPh>
-    <rPh sb="23" eb="25">
-      <t>コベツ</t>
-    </rPh>
-    <rPh sb="26" eb="28">
-      <t>ショリ</t>
-    </rPh>
-    <rPh sb="29" eb="31">
-      <t>ツイカ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[3-1，3-2共通]</t>
+    <rPh sb="8" eb="10">
+      <t>キョウツウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>タイマーが終了した時点で指定されたプロセスを実行</t>
+    <rPh sb="22" eb="24">
+      <t>ジッコウ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -2088,7 +2270,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2113,6 +2295,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -2128,13 +2313,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>73</xdr:row>
+      <xdr:row>77</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>33</xdr:col>
       <xdr:colOff>67412</xdr:colOff>
-      <xdr:row>88</xdr:row>
+      <xdr:row>92</xdr:row>
       <xdr:rowOff>28918</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -5249,6 +5434,44 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>419829</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>105149</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="図 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7743825" y="3771900"/>
+          <a:ext cx="5220429" cy="2676899"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5537,13 +5760,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:BU135"/>
+  <dimension ref="B2:BU142"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.25" defaultRowHeight="13.5"/>
   <cols>
-    <col min="2" max="2" width="2.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:71">
@@ -5573,7 +5798,7 @@
     </row>
     <row r="9" spans="2:71">
       <c r="C9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="10" spans="2:71">
@@ -5709,13 +5934,13 @@
       </c>
       <c r="AI21" s="1"/>
       <c r="AJ21" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="22" spans="2:36">
       <c r="AI22" s="1"/>
       <c r="AJ22" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="23" spans="2:36">
@@ -5743,385 +5968,406 @@
       </c>
     </row>
     <row r="27" spans="2:36">
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="C27" t="s">
+        <v>215</v>
+      </c>
       <c r="AI27" s="1"/>
     </row>
     <row r="28" spans="2:36">
-      <c r="B28">
-        <v>3</v>
-      </c>
       <c r="C28" t="s">
-        <v>34</v>
+        <v>218</v>
       </c>
       <c r="AI28" s="1"/>
     </row>
     <row r="29" spans="2:36">
       <c r="D29" t="s">
+        <v>124</v>
+      </c>
+      <c r="AI29" s="1"/>
+    </row>
+    <row r="30" spans="2:36">
+      <c r="AI30" s="1"/>
+    </row>
+    <row r="31" spans="2:36">
+      <c r="B31" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="C31" t="s">
+        <v>34</v>
+      </c>
+      <c r="AI31" s="1"/>
+    </row>
+    <row r="32" spans="2:36">
+      <c r="D32" t="s">
         <v>14</v>
       </c>
-      <c r="AI29" s="1"/>
-    </row>
-    <row r="30" spans="2:36">
-      <c r="D30" t="s">
-        <v>125</v>
-      </c>
-      <c r="AI30" s="1"/>
-    </row>
-    <row r="31" spans="2:36">
-      <c r="AI31" s="1"/>
-      <c r="AJ31" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="32" spans="2:36">
       <c r="AI32" s="1"/>
+      <c r="AJ32" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="33" spans="2:36">
-      <c r="B33">
-        <v>4</v>
-      </c>
-      <c r="C33" t="s">
-        <v>35</v>
-      </c>
       <c r="AI33" s="1"/>
     </row>
     <row r="34" spans="2:36">
-      <c r="D34" t="s">
-        <v>41</v>
+      <c r="B34" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="C34" t="s">
+        <v>216</v>
       </c>
       <c r="AI34" s="1"/>
-      <c r="AJ34" t="s">
-        <v>91</v>
-      </c>
     </row>
     <row r="35" spans="2:36">
       <c r="D35" t="s">
-        <v>96</v>
+        <v>219</v>
       </c>
       <c r="AI35" s="1"/>
       <c r="AJ35" t="s">
-        <v>112</v>
+        <v>217</v>
       </c>
     </row>
     <row r="36" spans="2:36">
       <c r="AI36" s="1"/>
-      <c r="AJ36" t="s">
-        <v>40</v>
-      </c>
     </row>
     <row r="37" spans="2:36">
+      <c r="B37">
+        <v>4</v>
+      </c>
+      <c r="C37" t="s">
+        <v>35</v>
+      </c>
       <c r="AI37" s="1"/>
     </row>
     <row r="38" spans="2:36">
-      <c r="B38">
-        <v>5</v>
-      </c>
-      <c r="C38" t="s">
-        <v>15</v>
+      <c r="D38" t="s">
+        <v>41</v>
       </c>
       <c r="AI38" s="1"/>
+      <c r="AJ38" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="39" spans="2:36">
       <c r="D39" t="s">
-        <v>16</v>
+        <v>96</v>
       </c>
       <c r="AI39" s="1"/>
       <c r="AJ39" t="s">
-        <v>190</v>
+        <v>112</v>
       </c>
     </row>
     <row r="40" spans="2:36">
-      <c r="D40" t="s">
-        <v>111</v>
-      </c>
       <c r="AI40" s="1"/>
       <c r="AJ40" t="s">
-        <v>191</v>
+        <v>40</v>
       </c>
     </row>
     <row r="41" spans="2:36">
-      <c r="D41" t="s">
-        <v>43</v>
-      </c>
       <c r="AI41" s="1"/>
-      <c r="AJ41" t="s">
-        <v>54</v>
-      </c>
     </row>
     <row r="42" spans="2:36">
+      <c r="B42">
+        <v>5</v>
+      </c>
+      <c r="C42" t="s">
+        <v>15</v>
+      </c>
       <c r="AI42" s="1"/>
-      <c r="AJ42" t="s">
-        <v>88</v>
-      </c>
     </row>
     <row r="43" spans="2:36">
+      <c r="D43" t="s">
+        <v>16</v>
+      </c>
       <c r="AI43" s="1"/>
       <c r="AJ43" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="44" spans="2:36">
+      <c r="D44" t="s">
+        <v>111</v>
+      </c>
       <c r="AI44" s="1"/>
       <c r="AJ44" t="s">
-        <v>89</v>
+        <v>189</v>
       </c>
     </row>
     <row r="45" spans="2:36">
+      <c r="D45" t="s">
+        <v>43</v>
+      </c>
       <c r="AI45" s="1"/>
       <c r="AJ45" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="46" spans="2:36">
+      <c r="AI46" s="1"/>
+      <c r="AJ46" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="47" spans="2:36">
+      <c r="AI47" s="1"/>
+      <c r="AJ47" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="48" spans="2:36">
+      <c r="AI48" s="1"/>
+      <c r="AJ48" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="49" spans="2:36">
+      <c r="AI49" s="1"/>
+      <c r="AJ49" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="46" spans="2:36">
-      <c r="B46">
+    <row r="50" spans="2:36">
+      <c r="B50">
         <v>6</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C50" t="s">
         <v>17</v>
-      </c>
-      <c r="AI46" s="1"/>
-    </row>
-    <row r="47" spans="2:36">
-      <c r="D47" t="s">
-        <v>48</v>
-      </c>
-      <c r="AI47" s="1"/>
-    </row>
-    <row r="48" spans="2:36">
-      <c r="D48" t="s">
-        <v>188</v>
-      </c>
-      <c r="AI48" s="1"/>
-    </row>
-    <row r="49" spans="2:36">
-      <c r="D49" t="s">
-        <v>189</v>
-      </c>
-      <c r="AI49" s="1"/>
-    </row>
-    <row r="50" spans="2:36">
-      <c r="D50" t="s">
-        <v>45</v>
       </c>
       <c r="AI50" s="1"/>
     </row>
     <row r="51" spans="2:36">
       <c r="D51" t="s">
-        <v>110</v>
+        <v>48</v>
       </c>
       <c r="AI51" s="1"/>
     </row>
     <row r="52" spans="2:36">
       <c r="D52" t="s">
-        <v>18</v>
+        <v>186</v>
       </c>
       <c r="AI52" s="1"/>
-      <c r="AJ52" t="s">
-        <v>109</v>
-      </c>
     </row>
     <row r="53" spans="2:36">
       <c r="D53" t="s">
-        <v>53</v>
+        <v>187</v>
       </c>
       <c r="AI53" s="1"/>
-      <c r="AJ53" t="s">
-        <v>108</v>
-      </c>
     </row>
     <row r="54" spans="2:36">
+      <c r="D54" t="s">
+        <v>45</v>
+      </c>
       <c r="AI54" s="1"/>
-      <c r="AJ54" t="s">
-        <v>193</v>
-      </c>
     </row>
     <row r="55" spans="2:36">
-      <c r="B55">
-        <v>7</v>
-      </c>
-      <c r="C55" t="s">
-        <v>19</v>
+      <c r="D55" t="s">
+        <v>110</v>
       </c>
       <c r="AI55" s="1"/>
     </row>
     <row r="56" spans="2:36">
       <c r="D56" t="s">
-        <v>52</v>
+        <v>18</v>
       </c>
       <c r="AI56" s="1"/>
       <c r="AJ56" t="s">
-        <v>47</v>
+        <v>109</v>
       </c>
     </row>
     <row r="57" spans="2:36">
+      <c r="D57" t="s">
+        <v>53</v>
+      </c>
       <c r="AI57" s="1"/>
+      <c r="AJ57" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="58" spans="2:36">
-      <c r="B58">
-        <v>8</v>
-      </c>
-      <c r="C58" t="s">
-        <v>44</v>
-      </c>
       <c r="AI58" s="1"/>
+      <c r="AJ58" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="59" spans="2:36">
-      <c r="D59" t="s">
-        <v>49</v>
+      <c r="B59">
+        <v>7</v>
+      </c>
+      <c r="C59" t="s">
+        <v>19</v>
       </c>
       <c r="AI59" s="1"/>
-      <c r="AJ59" t="s">
-        <v>87</v>
-      </c>
     </row>
     <row r="60" spans="2:36">
       <c r="D60" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="AI60" s="1"/>
+      <c r="AJ60" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="61" spans="2:36">
-      <c r="D61" t="s">
-        <v>56</v>
-      </c>
       <c r="AI61" s="1"/>
-      <c r="AJ61" t="s">
-        <v>104</v>
-      </c>
     </row>
     <row r="62" spans="2:36">
-      <c r="D62" t="s">
-        <v>98</v>
+      <c r="B62">
+        <v>8</v>
+      </c>
+      <c r="C62" t="s">
+        <v>44</v>
       </c>
       <c r="AI62" s="1"/>
     </row>
     <row r="63" spans="2:36">
+      <c r="D63" t="s">
+        <v>49</v>
+      </c>
       <c r="AI63" s="1"/>
       <c r="AJ63" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
     </row>
     <row r="64" spans="2:36">
+      <c r="D64" t="s">
+        <v>57</v>
+      </c>
       <c r="AI64" s="1"/>
-      <c r="AJ64" t="s">
-        <v>103</v>
-      </c>
     </row>
     <row r="65" spans="2:73">
+      <c r="D65" t="s">
+        <v>56</v>
+      </c>
       <c r="AI65" s="1"/>
       <c r="AJ65" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="66" spans="2:73">
+      <c r="D66" t="s">
+        <v>98</v>
+      </c>
       <c r="AI66" s="1"/>
-      <c r="AJ66" t="s">
-        <v>106</v>
-      </c>
     </row>
     <row r="67" spans="2:73">
       <c r="AI67" s="1"/>
+      <c r="AJ67" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="68" spans="2:73">
       <c r="AI68" s="1"/>
+      <c r="AJ68" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="69" spans="2:73">
-      <c r="AI69" s="2"/>
+      <c r="AI69" s="1"/>
+      <c r="AJ69" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="70" spans="2:73">
-      <c r="B70" s="5"/>
-      <c r="C70" s="5"/>
-      <c r="D70" s="5"/>
-      <c r="E70" s="5"/>
-      <c r="F70" s="5"/>
-      <c r="G70" s="5"/>
-      <c r="H70" s="5"/>
-      <c r="I70" s="5"/>
-      <c r="J70" s="5"/>
-      <c r="K70" s="5"/>
-      <c r="L70" s="5"/>
-      <c r="M70" s="5"/>
-      <c r="N70" s="5"/>
-      <c r="O70" s="5"/>
-      <c r="P70" s="5"/>
-      <c r="Q70" s="5"/>
-      <c r="R70" s="5"/>
-      <c r="S70" s="5"/>
-      <c r="T70" s="5"/>
-      <c r="U70" s="5"/>
-      <c r="V70" s="5"/>
-      <c r="W70" s="5"/>
-      <c r="X70" s="5"/>
-      <c r="Y70" s="5"/>
-      <c r="Z70" s="5"/>
-      <c r="AA70" s="5"/>
-      <c r="AB70" s="5"/>
-      <c r="AC70" s="5"/>
-      <c r="AD70" s="5"/>
-      <c r="AE70" s="5"/>
-      <c r="AF70" s="5"/>
-      <c r="AG70" s="5"/>
-      <c r="AH70" s="5"/>
-      <c r="AI70" s="5"/>
-      <c r="AJ70" s="5"/>
-      <c r="AK70" s="5"/>
-      <c r="AL70" s="5"/>
-      <c r="AM70" s="5"/>
-      <c r="AN70" s="5"/>
-      <c r="AO70" s="5"/>
-      <c r="AP70" s="5"/>
-      <c r="AQ70" s="5"/>
-      <c r="AR70" s="5"/>
-      <c r="AS70" s="5"/>
-      <c r="AT70" s="5"/>
-      <c r="AU70" s="5"/>
-      <c r="AV70" s="5"/>
-      <c r="AW70" s="5"/>
-      <c r="AX70" s="5"/>
-      <c r="AY70" s="5"/>
-      <c r="AZ70" s="5"/>
-      <c r="BA70" s="5"/>
-      <c r="BB70" s="5"/>
-      <c r="BC70" s="5"/>
-      <c r="BD70" s="5"/>
-      <c r="BE70" s="5"/>
-      <c r="BF70" s="5"/>
-      <c r="BG70" s="5"/>
-      <c r="BH70" s="5"/>
-      <c r="BI70" s="5"/>
-      <c r="BJ70" s="5"/>
-      <c r="BK70" s="5"/>
-      <c r="BL70" s="5"/>
-      <c r="BM70" s="5"/>
-      <c r="BN70" s="5"/>
-      <c r="BO70" s="5"/>
-      <c r="BP70" s="5"/>
-      <c r="BQ70" s="5"/>
-      <c r="BR70" s="5"/>
-      <c r="BS70" s="5"/>
-      <c r="BT70" s="5"/>
-      <c r="BU70" s="5"/>
+      <c r="AI70" s="1"/>
+      <c r="AJ70" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="71" spans="2:73">
+      <c r="AI71" s="1"/>
     </row>
     <row r="72" spans="2:73">
-      <c r="B72" t="s">
+      <c r="AI72" s="1"/>
+    </row>
+    <row r="73" spans="2:73">
+      <c r="AI73" s="2"/>
+    </row>
+    <row r="74" spans="2:73">
+      <c r="B74" s="5"/>
+      <c r="C74" s="5"/>
+      <c r="D74" s="5"/>
+      <c r="E74" s="5"/>
+      <c r="F74" s="5"/>
+      <c r="G74" s="5"/>
+      <c r="H74" s="5"/>
+      <c r="I74" s="5"/>
+      <c r="J74" s="5"/>
+      <c r="K74" s="5"/>
+      <c r="L74" s="5"/>
+      <c r="M74" s="5"/>
+      <c r="N74" s="5"/>
+      <c r="O74" s="5"/>
+      <c r="P74" s="5"/>
+      <c r="Q74" s="5"/>
+      <c r="R74" s="5"/>
+      <c r="S74" s="5"/>
+      <c r="T74" s="5"/>
+      <c r="U74" s="5"/>
+      <c r="V74" s="5"/>
+      <c r="W74" s="5"/>
+      <c r="X74" s="5"/>
+      <c r="Y74" s="5"/>
+      <c r="Z74" s="5"/>
+      <c r="AA74" s="5"/>
+      <c r="AB74" s="5"/>
+      <c r="AC74" s="5"/>
+      <c r="AD74" s="5"/>
+      <c r="AE74" s="5"/>
+      <c r="AF74" s="5"/>
+      <c r="AG74" s="5"/>
+      <c r="AH74" s="5"/>
+      <c r="AI74" s="5"/>
+      <c r="AJ74" s="5"/>
+      <c r="AK74" s="5"/>
+      <c r="AL74" s="5"/>
+      <c r="AM74" s="5"/>
+      <c r="AN74" s="5"/>
+      <c r="AO74" s="5"/>
+      <c r="AP74" s="5"/>
+      <c r="AQ74" s="5"/>
+      <c r="AR74" s="5"/>
+      <c r="AS74" s="5"/>
+      <c r="AT74" s="5"/>
+      <c r="AU74" s="5"/>
+      <c r="AV74" s="5"/>
+      <c r="AW74" s="5"/>
+      <c r="AX74" s="5"/>
+      <c r="AY74" s="5"/>
+      <c r="AZ74" s="5"/>
+      <c r="BA74" s="5"/>
+      <c r="BB74" s="5"/>
+      <c r="BC74" s="5"/>
+      <c r="BD74" s="5"/>
+      <c r="BE74" s="5"/>
+      <c r="BF74" s="5"/>
+      <c r="BG74" s="5"/>
+      <c r="BH74" s="5"/>
+      <c r="BI74" s="5"/>
+      <c r="BJ74" s="5"/>
+      <c r="BK74" s="5"/>
+      <c r="BL74" s="5"/>
+      <c r="BM74" s="5"/>
+      <c r="BN74" s="5"/>
+      <c r="BO74" s="5"/>
+      <c r="BP74" s="5"/>
+      <c r="BQ74" s="5"/>
+      <c r="BR74" s="5"/>
+      <c r="BS74" s="5"/>
+      <c r="BT74" s="5"/>
+      <c r="BU74" s="5"/>
+    </row>
+    <row r="76" spans="2:73">
+      <c r="B76" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="73" spans="2:73">
-      <c r="C73" t="s">
+    <row r="77" spans="2:73">
+      <c r="C77" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="74" spans="2:73">
-      <c r="AI74" s="2"/>
-    </row>
-    <row r="75" spans="2:73">
-      <c r="AI75" s="2"/>
-    </row>
-    <row r="76" spans="2:73">
-      <c r="AI76" s="2"/>
-    </row>
-    <row r="77" spans="2:73">
-      <c r="AI77" s="2"/>
     </row>
     <row r="78" spans="2:73">
       <c r="AI78" s="2"/>
@@ -6163,226 +6409,258 @@
       <c r="AI90" s="2"/>
     </row>
     <row r="91" spans="2:35">
-      <c r="B91" t="s">
+      <c r="AI91" s="2"/>
+    </row>
+    <row r="92" spans="2:35">
+      <c r="AI92" s="2"/>
+    </row>
+    <row r="93" spans="2:35">
+      <c r="AI93" s="2"/>
+    </row>
+    <row r="94" spans="2:35">
+      <c r="AI94" s="2"/>
+    </row>
+    <row r="95" spans="2:35">
+      <c r="B95" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="92" spans="2:35">
-      <c r="C92" t="s">
+    <row r="96" spans="2:35">
+      <c r="C96" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="93" spans="2:35">
-      <c r="C93" t="s">
+    <row r="97" spans="2:56">
+      <c r="C97" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="94" spans="2:35">
-      <c r="C94" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="95" spans="2:35">
-      <c r="C95" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="97" spans="2:56">
-      <c r="B97" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="98" spans="2:56">
       <c r="C98" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="99" spans="2:56">
       <c r="C99" t="s">
-        <v>28</v>
-      </c>
-      <c r="BB99" s="1"/>
-      <c r="BC99" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="100" spans="2:56">
-      <c r="C100" t="s">
-        <v>46</v>
-      </c>
-      <c r="BB100" s="1"/>
-      <c r="BD100" t="s">
-        <v>119</v>
+        <v>25</v>
       </c>
     </row>
     <row r="101" spans="2:56">
-      <c r="C101" t="s">
-        <v>58</v>
-      </c>
-      <c r="BB101" s="1"/>
-      <c r="BD101" t="s">
-        <v>120</v>
+      <c r="B101" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="102" spans="2:56">
       <c r="C102" t="s">
-        <v>33</v>
-      </c>
-      <c r="BB102" s="1"/>
-      <c r="BD102" t="s">
-        <v>121</v>
+        <v>27</v>
       </c>
     </row>
     <row r="103" spans="2:56">
+      <c r="C103" t="s">
+        <v>28</v>
+      </c>
       <c r="BB103" s="1"/>
-      <c r="BD103" t="s">
+      <c r="BC103" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="104" spans="2:56">
-      <c r="B104" t="s">
-        <v>29</v>
+      <c r="C104" t="s">
+        <v>46</v>
       </c>
       <c r="BB104" s="1"/>
+      <c r="BD104" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="105" spans="2:56">
       <c r="C105" t="s">
-        <v>196</v>
+        <v>58</v>
       </c>
       <c r="BB105" s="1"/>
+      <c r="BD105" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="106" spans="2:56">
       <c r="C106" t="s">
-        <v>195</v>
+        <v>33</v>
+      </c>
+      <c r="BB106" s="1"/>
+      <c r="BD106" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="107" spans="2:56">
-      <c r="C107" t="s">
+      <c r="BB107" s="1"/>
+      <c r="BD107" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="108" spans="2:56">
+      <c r="B108" t="s">
+        <v>29</v>
+      </c>
+      <c r="BB108" s="1"/>
+    </row>
+    <row r="109" spans="2:56">
+      <c r="C109" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="109" spans="2:56">
-      <c r="B109" t="s">
-        <v>30</v>
-      </c>
+      <c r="BB109" s="1"/>
     </row>
     <row r="110" spans="2:56">
       <c r="C110" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="111" spans="2:56">
       <c r="C111" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="112" spans="2:56">
-      <c r="C112" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="113" spans="3:3">
-      <c r="C113" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="113" spans="2:3">
+      <c r="B113" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="114" spans="2:3">
+      <c r="C114" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="115" spans="2:3">
+      <c r="C115" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="116" spans="2:3">
+      <c r="C116" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="117" spans="2:3">
+      <c r="C117" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="118" spans="2:3">
+      <c r="C118" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="119" spans="2:3">
+      <c r="C119" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="120" spans="2:3">
+      <c r="C120" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="121" spans="2:3">
+      <c r="C121" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="122" spans="2:3">
+      <c r="C122" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="114" spans="3:3">
-      <c r="C114" t="s">
+    <row r="123" spans="2:3">
+      <c r="C123" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="124" spans="2:3">
+      <c r="C124" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="125" spans="2:3">
+      <c r="C125" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="126" spans="2:3">
+      <c r="C126" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="127" spans="2:3">
+      <c r="C127" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="115" spans="3:3">
-      <c r="C115" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="116" spans="3:3">
-      <c r="C116" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="117" spans="3:3">
-      <c r="C117" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="118" spans="3:3">
-      <c r="C118" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="119" spans="3:3">
-      <c r="C119" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="120" spans="3:3">
-      <c r="C120" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="121" spans="3:3">
-      <c r="C121" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="122" spans="3:3">
-      <c r="C122" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="123" spans="3:3">
-      <c r="C123" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="124" spans="3:3">
-      <c r="C124" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="125" spans="3:3">
-      <c r="C125" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="126" spans="3:3">
-      <c r="C126" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="128" spans="3:3">
+    <row r="128" spans="2:3">
       <c r="C128" t="s">
-        <v>199</v>
+        <v>210</v>
       </c>
     </row>
     <row r="129" spans="3:3">
       <c r="C129" t="s">
-        <v>37</v>
+        <v>211</v>
       </c>
     </row>
     <row r="130" spans="3:3">
       <c r="C130" t="s">
-        <v>116</v>
+        <v>196</v>
       </c>
     </row>
     <row r="131" spans="3:3">
       <c r="C131" t="s">
-        <v>95</v>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="132" spans="3:3">
+      <c r="C132" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="133" spans="3:3">
       <c r="C133" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="134" spans="3:3">
       <c r="C134" t="s">
-        <v>31</v>
+        <v>211</v>
       </c>
     </row>
     <row r="135" spans="3:3">
       <c r="C135" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="136" spans="3:3">
+      <c r="C136" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="137" spans="3:3">
+      <c r="C137" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="138" spans="3:3">
+      <c r="C138" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="140" spans="3:3">
+      <c r="C140" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="141" spans="3:3">
+      <c r="C141" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="142" spans="3:3">
+      <c r="C142" t="s">
         <v>20</v>
       </c>
     </row>
@@ -6575,246 +6853,246 @@
   <sheetData>
     <row r="1" spans="2:101">
       <c r="CW1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" spans="2:101">
       <c r="B2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="AP2" s="6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="2:101" ht="15">
       <c r="B5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="BV5" s="7" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="7" spans="2:101">
       <c r="B7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="2:101">
       <c r="B8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="2:101">
       <c r="B9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="2:101">
       <c r="B11" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="12" spans="2:101">
       <c r="B12" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="13" spans="2:101">
       <c r="B13" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14" spans="2:101">
       <c r="B14" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="15" spans="2:101">
       <c r="B15" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="16" spans="2:101">
       <c r="B16" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="17" spans="2:72">
       <c r="B17" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="18" spans="2:72">
       <c r="B18" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="19" spans="2:72">
       <c r="B19" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="20" spans="2:72">
       <c r="B20" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="22" spans="2:72">
       <c r="B22" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="23" spans="2:72">
       <c r="B23" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="24" spans="2:72">
       <c r="B24" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="25" spans="2:72">
       <c r="B25" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="BT25" s="6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="27" spans="2:72">
       <c r="B27" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="28" spans="2:72">
       <c r="B28" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="29" spans="2:72">
       <c r="B29" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="31" spans="2:72">
       <c r="B31" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="32" spans="2:72">
       <c r="B32" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="33" spans="2:42">
       <c r="B33" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="35" spans="2:42">
       <c r="B35" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="36" spans="2:42">
       <c r="B36" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="37" spans="2:42">
       <c r="B37" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="39" spans="2:42">
       <c r="B39" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="40" spans="2:42">
       <c r="B40" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="41" spans="2:42">
       <c r="B41" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="42" spans="2:42">
       <c r="AP42" s="6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="43" spans="2:42">
       <c r="B43" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="44" spans="2:42">
       <c r="B44" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="45" spans="2:42">
       <c r="B45" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="47" spans="2:42">
       <c r="B47" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="48" spans="2:42">
       <c r="B48" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="49" spans="2:3">
       <c r="B49" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="50" spans="2:3">
       <c r="B50" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="53" spans="2:3">
       <c r="B53" s="6" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="54" spans="2:3">
       <c r="C54" s="6" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="55" spans="2:3">
       <c r="C55" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="56" spans="2:3">
       <c r="C56" s="6" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="58" spans="2:3">
       <c r="C58" s="6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="59" spans="2:3">
       <c r="C59" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="60" spans="2:3">
       <c r="C60" s="6" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -6827,9 +7105,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:L11"/>
+  <dimension ref="B2:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
@@ -6849,7 +7129,7 @@
         <v>6</v>
       </c>
       <c r="L3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="2:12">
@@ -6873,7 +7153,7 @@
         <v>240813</v>
       </c>
       <c r="C6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="2:12">
@@ -6881,7 +7161,7 @@
         <v>240813</v>
       </c>
       <c r="C7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="2:12">
@@ -6889,7 +7169,7 @@
         <v>240813</v>
       </c>
       <c r="C8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="2:12">
@@ -6897,7 +7177,7 @@
         <v>240813</v>
       </c>
       <c r="C9" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="2:12">
@@ -6905,7 +7185,7 @@
         <v>240813</v>
       </c>
       <c r="C10" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" spans="2:12">
@@ -6913,7 +7193,44 @@
         <v>240813</v>
       </c>
       <c r="C11" t="s">
-        <v>183</v>
+        <v>181</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12">
+      <c r="B12">
+        <v>240816</v>
+      </c>
+      <c r="C12" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12">
+      <c r="B13">
+        <v>240816</v>
+      </c>
+      <c r="C13" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12">
+      <c r="B14">
+        <v>240816</v>
+      </c>
+      <c r="C14" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12">
+      <c r="B15">
+        <v>240816</v>
+      </c>
+      <c r="C15" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="21" spans="12:12">
+      <c r="L21" t="s">
+        <v>205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>